<commit_message>
Fixed last layer, and norm layers
</commit_message>
<xml_diff>
--- a/tasks results.xlsx
+++ b/tasks results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="task 2" sheetId="1" r:id="rId1"/>
@@ -398,64 +398,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2.2949999999999999</c:v>
+                  <c:v>2.278</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2799999999999998</c:v>
+                  <c:v>2.2389999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2589999999999999</c:v>
+                  <c:v>2.1789999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2290000000000001</c:v>
+                  <c:v>2.0670000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1869999999999998</c:v>
+                  <c:v>1.827</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.113</c:v>
+                  <c:v>1.3819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0110000000000001</c:v>
+                  <c:v>0.95199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.863</c:v>
+                  <c:v>0.69499999999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7110000000000001</c:v>
+                  <c:v>0.56599999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5780000000000001</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.496</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.43</c:v>
+                  <c:v>0.39900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3819999999999999</c:v>
+                  <c:v>0.36899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.325</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3029999999999999</c:v>
+                  <c:v>0.32800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.2629999999999999</c:v>
+                  <c:v>0.311</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.26</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.214</c:v>
+                  <c:v>0.29399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.216</c:v>
+                  <c:v>0.27600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.21</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -470,11 +470,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="403562840"/>
-        <c:axId val="403568720"/>
+        <c:axId val="524164896"/>
+        <c:axId val="524157056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="403562840"/>
+        <c:axId val="524164896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,12 +587,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403568720"/>
+        <c:crossAx val="524157056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="403568720"/>
+        <c:axId val="524157056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403562840"/>
+        <c:crossAx val="524164896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -944,64 +944,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.35</c:v>
+                  <c:v>2.2930000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48699999999999999</c:v>
+                  <c:v>2.2749999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33300000000000002</c:v>
+                  <c:v>2.2519999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27100000000000002</c:v>
+                  <c:v>2.2189999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.224</c:v>
+                  <c:v>2.161</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>2.0550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.186</c:v>
+                  <c:v>1.8380000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16600000000000001</c:v>
+                  <c:v>1.4750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.158</c:v>
+                  <c:v>1.0940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14399999999999999</c:v>
+                  <c:v>0.84799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14099999999999999</c:v>
+                  <c:v>0.71399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13300000000000001</c:v>
+                  <c:v>0.61299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.126</c:v>
+                  <c:v>0.55800000000000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11899999999999999</c:v>
+                  <c:v>0.495</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.108</c:v>
+                  <c:v>0.47299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.109</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.105</c:v>
+                  <c:v>0.41299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.8000000000000004E-2</c:v>
+                  <c:v>0.39400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.7000000000000003E-2</c:v>
+                  <c:v>0.36599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.09</c:v>
+                  <c:v>0.36599999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1016,11 +1016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404886920"/>
-        <c:axId val="404887312"/>
+        <c:axId val="530979392"/>
+        <c:axId val="530984880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404886920"/>
+        <c:axId val="530979392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,12 +1133,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404887312"/>
+        <c:crossAx val="530984880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404887312"/>
+        <c:axId val="530984880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +1251,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404886920"/>
+        <c:crossAx val="530979392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2749,8 +2749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,7 +2771,7 @@
         <v>250</v>
       </c>
       <c r="B2" s="2">
-        <v>2.2949999999999999</v>
+        <v>2.278</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>500</v>
       </c>
       <c r="B3" s="1">
-        <v>2.2799999999999998</v>
+        <v>2.2389999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>750</v>
       </c>
       <c r="B4" s="1">
-        <v>2.2589999999999999</v>
+        <v>2.1789999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>1000</v>
       </c>
       <c r="B5" s="1">
-        <v>2.2290000000000001</v>
+        <v>2.0670000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2803,7 +2803,7 @@
         <v>1250</v>
       </c>
       <c r="B6" s="1">
-        <v>2.1869999999999998</v>
+        <v>1.827</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
         <v>1500</v>
       </c>
       <c r="B7" s="1">
-        <v>2.113</v>
+        <v>1.3819999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>1750</v>
       </c>
       <c r="B8" s="1">
-        <v>2.0110000000000001</v>
+        <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2827,7 +2827,7 @@
         <v>2000</v>
       </c>
       <c r="B9" s="1">
-        <v>1.863</v>
+        <v>0.69499999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2835,7 +2835,7 @@
         <v>2250</v>
       </c>
       <c r="B10" s="1">
-        <v>1.7110000000000001</v>
+        <v>0.56599999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2843,7 +2843,7 @@
         <v>2500</v>
       </c>
       <c r="B11" s="1">
-        <v>1.5780000000000001</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2851,7 +2851,7 @@
         <v>2750</v>
       </c>
       <c r="B12" s="1">
-        <v>1.496</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2859,7 +2859,7 @@
         <v>3000</v>
       </c>
       <c r="B13" s="1">
-        <v>1.43</v>
+        <v>0.39900000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2867,7 +2867,7 @@
         <v>3250</v>
       </c>
       <c r="B14" s="1">
-        <v>1.3819999999999999</v>
+        <v>0.36899999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2875,7 +2875,7 @@
         <v>3500</v>
       </c>
       <c r="B15" s="1">
-        <v>1.325</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
         <v>3750</v>
       </c>
       <c r="B16" s="1">
-        <v>1.3029999999999999</v>
+        <v>0.32800000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>4000</v>
       </c>
       <c r="B17" s="1">
-        <v>1.2629999999999999</v>
+        <v>0.311</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2899,7 +2899,7 @@
         <v>4250</v>
       </c>
       <c r="B18" s="1">
-        <v>1.26</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2907,7 +2907,7 @@
         <v>4500</v>
       </c>
       <c r="B19" s="1">
-        <v>1.214</v>
+        <v>0.29399999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2915,7 +2915,7 @@
         <v>4750</v>
       </c>
       <c r="B20" s="1">
-        <v>1.216</v>
+        <v>0.27600000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2923,7 +2923,7 @@
         <v>5000</v>
       </c>
       <c r="B21" s="1">
-        <v>1.21</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2932,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="6">
-        <v>0.57809999999999995</v>
+        <v>0.92600000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -2946,8 +2946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,7 +2968,7 @@
         <v>250</v>
       </c>
       <c r="B2" s="2">
-        <v>1.35</v>
+        <v>2.2930000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>500</v>
       </c>
       <c r="B3" s="1">
-        <v>0.48699999999999999</v>
+        <v>2.2749999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2984,7 +2984,7 @@
         <v>750</v>
       </c>
       <c r="B4" s="1">
-        <v>0.33300000000000002</v>
+        <v>2.2519999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2992,7 +2992,7 @@
         <v>1000</v>
       </c>
       <c r="B5" s="1">
-        <v>0.27100000000000002</v>
+        <v>2.2189999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
         <v>1250</v>
       </c>
       <c r="B6" s="1">
-        <v>0.224</v>
+        <v>2.161</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
         <v>1500</v>
       </c>
       <c r="B7" s="1">
-        <v>0.20799999999999999</v>
+        <v>2.0550000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <v>1750</v>
       </c>
       <c r="B8" s="1">
-        <v>0.186</v>
+        <v>1.8380000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3024,7 +3024,7 @@
         <v>2000</v>
       </c>
       <c r="B9" s="1">
-        <v>0.16600000000000001</v>
+        <v>1.4750000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>2250</v>
       </c>
       <c r="B10" s="1">
-        <v>0.158</v>
+        <v>1.0940000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>2500</v>
       </c>
       <c r="B11" s="1">
-        <v>0.14399999999999999</v>
+        <v>0.84799999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
         <v>2750</v>
       </c>
       <c r="B12" s="1">
-        <v>0.14099999999999999</v>
+        <v>0.71399999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
         <v>3000</v>
       </c>
       <c r="B13" s="1">
-        <v>0.13300000000000001</v>
+        <v>0.61299999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>3250</v>
       </c>
       <c r="B14" s="1">
-        <v>0.126</v>
+        <v>0.55800000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>3500</v>
       </c>
       <c r="B15" s="1">
-        <v>0.11899999999999999</v>
+        <v>0.495</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>3750</v>
       </c>
       <c r="B16" s="1">
-        <v>0.108</v>
+        <v>0.47299999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>4000</v>
       </c>
       <c r="B17" s="1">
-        <v>0.109</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>4250</v>
       </c>
       <c r="B18" s="1">
-        <v>0.105</v>
+        <v>0.41299999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3104,7 @@
         <v>4500</v>
       </c>
       <c r="B19" s="1">
-        <v>9.8000000000000004E-2</v>
+        <v>0.39400000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>4750</v>
       </c>
       <c r="B20" s="1">
-        <v>9.7000000000000003E-2</v>
+        <v>0.36599999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>5000</v>
       </c>
       <c r="B21" s="1">
-        <v>0.09</v>
+        <v>0.36599999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3129,7 +3129,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="6">
-        <v>0.64280000000000004</v>
+        <v>0.91759999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote report, added zip for submission
</commit_message>
<xml_diff>
--- a/tasks results.xlsx
+++ b/tasks results.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="task 2" sheetId="1" r:id="rId1"/>
     <sheet name="task 3" sheetId="3" r:id="rId2"/>
+    <sheet name="task 4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Iteration</t>
   </si>
@@ -34,6 +35,9 @@
   </si>
   <si>
     <t>Test Accuracy</t>
+  </si>
+  <si>
+    <t>Validation Accuracy</t>
   </si>
 </sst>
 </file>
@@ -167,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,6 +194,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,11 +480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="524164896"/>
-        <c:axId val="524157056"/>
+        <c:axId val="431083296"/>
+        <c:axId val="431082512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="524164896"/>
+        <c:axId val="431083296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,12 +597,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="524157056"/>
+        <c:crossAx val="431082512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="524157056"/>
+        <c:axId val="431082512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +715,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="524164896"/>
+        <c:crossAx val="431083296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1016,11 +1026,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="530979392"/>
-        <c:axId val="530984880"/>
+        <c:axId val="431080160"/>
+        <c:axId val="431086824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="530979392"/>
+        <c:axId val="431080160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,12 +1143,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530984880"/>
+        <c:crossAx val="431086824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="530984880"/>
+        <c:axId val="431086824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +1261,541 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="530979392"/>
+        <c:crossAx val="431080160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Task 3 - Cost as Function of Iteration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'task 4'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'task 4'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'task 4'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3039999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.294</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.306</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2959999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.298</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.3029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.3119999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="435552632"/>
+        <c:axId val="435551456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="435552632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1"/>
+                  <a:t>Iteration Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435551456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435551456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1"/>
+                  <a:t>Cost</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435552632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1380,6 +1924,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1897,6 +2481,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2460,6 +3560,43 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
       <xdr:row>22</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2750,7 +3887,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,7 +3907,7 @@
       <c r="A2" s="2">
         <v>250</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="9">
         <v>2.278</v>
       </c>
     </row>
@@ -2778,7 +3915,7 @@
       <c r="A3" s="1">
         <v>500</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="10">
         <v>2.2389999999999999</v>
       </c>
     </row>
@@ -2786,7 +3923,7 @@
       <c r="A4" s="1">
         <v>750</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="10">
         <v>2.1789999999999998</v>
       </c>
     </row>
@@ -2794,7 +3931,7 @@
       <c r="A5" s="1">
         <v>1000</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="10">
         <v>2.0670000000000002</v>
       </c>
     </row>
@@ -2802,7 +3939,7 @@
       <c r="A6" s="1">
         <v>1250</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="10">
         <v>1.827</v>
       </c>
     </row>
@@ -2810,7 +3947,7 @@
       <c r="A7" s="1">
         <v>1500</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="10">
         <v>1.3819999999999999</v>
       </c>
     </row>
@@ -2818,7 +3955,7 @@
       <c r="A8" s="1">
         <v>1750</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="10">
         <v>0.95199999999999996</v>
       </c>
     </row>
@@ -2826,7 +3963,7 @@
       <c r="A9" s="1">
         <v>2000</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="10">
         <v>0.69499999999999995</v>
       </c>
     </row>
@@ -2834,7 +3971,7 @@
       <c r="A10" s="1">
         <v>2250</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="10">
         <v>0.56599999999999995</v>
       </c>
     </row>
@@ -2842,7 +3979,7 @@
       <c r="A11" s="1">
         <v>2500</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="10">
         <v>0.48</v>
       </c>
     </row>
@@ -2850,7 +3987,7 @@
       <c r="A12" s="1">
         <v>2750</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="10">
         <v>0.44</v>
       </c>
     </row>
@@ -2858,7 +3995,7 @@
       <c r="A13" s="1">
         <v>3000</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="10">
         <v>0.39900000000000002</v>
       </c>
     </row>
@@ -2866,7 +4003,7 @@
       <c r="A14" s="1">
         <v>3250</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="10">
         <v>0.36899999999999999</v>
       </c>
     </row>
@@ -2874,7 +4011,7 @@
       <c r="A15" s="1">
         <v>3500</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="10">
         <v>0.35</v>
       </c>
     </row>
@@ -2882,7 +4019,7 @@
       <c r="A16" s="1">
         <v>3750</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="10">
         <v>0.32800000000000001</v>
       </c>
     </row>
@@ -2890,7 +4027,7 @@
       <c r="A17" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="10">
         <v>0.311</v>
       </c>
     </row>
@@ -2898,7 +4035,7 @@
       <c r="A18" s="1">
         <v>4250</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="10">
         <v>0.31</v>
       </c>
     </row>
@@ -2906,7 +4043,7 @@
       <c r="A19" s="1">
         <v>4500</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="10">
         <v>0.29399999999999998</v>
       </c>
     </row>
@@ -2914,7 +4051,7 @@
       <c r="A20" s="1">
         <v>4750</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="10">
         <v>0.27600000000000002</v>
       </c>
     </row>
@@ -2922,7 +4059,7 @@
       <c r="A21" s="1">
         <v>5000</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="10">
         <v>0.27</v>
       </c>
     </row>
@@ -2947,7 +4084,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,7 +4104,7 @@
       <c r="A2" s="2">
         <v>250</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="9">
         <v>2.2930000000000001</v>
       </c>
     </row>
@@ -2975,7 +4112,7 @@
       <c r="A3" s="1">
         <v>500</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="10">
         <v>2.2749999999999999</v>
       </c>
     </row>
@@ -2983,7 +4120,7 @@
       <c r="A4" s="1">
         <v>750</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="10">
         <v>2.2519999999999998</v>
       </c>
     </row>
@@ -2991,7 +4128,7 @@
       <c r="A5" s="1">
         <v>1000</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="10">
         <v>2.2189999999999999</v>
       </c>
     </row>
@@ -2999,7 +4136,7 @@
       <c r="A6" s="1">
         <v>1250</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="10">
         <v>2.161</v>
       </c>
     </row>
@@ -3007,7 +4144,7 @@
       <c r="A7" s="1">
         <v>1500</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="10">
         <v>2.0550000000000002</v>
       </c>
     </row>
@@ -3015,7 +4152,7 @@
       <c r="A8" s="1">
         <v>1750</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="10">
         <v>1.8380000000000001</v>
       </c>
     </row>
@@ -3023,7 +4160,7 @@
       <c r="A9" s="1">
         <v>2000</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="10">
         <v>1.4750000000000001</v>
       </c>
     </row>
@@ -3031,7 +4168,7 @@
       <c r="A10" s="1">
         <v>2250</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="10">
         <v>1.0940000000000001</v>
       </c>
     </row>
@@ -3039,7 +4176,7 @@
       <c r="A11" s="1">
         <v>2500</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="10">
         <v>0.84799999999999998</v>
       </c>
     </row>
@@ -3047,7 +4184,7 @@
       <c r="A12" s="1">
         <v>2750</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="10">
         <v>0.71399999999999997</v>
       </c>
     </row>
@@ -3055,7 +4192,7 @@
       <c r="A13" s="1">
         <v>3000</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="10">
         <v>0.61299999999999999</v>
       </c>
     </row>
@@ -3063,7 +4200,7 @@
       <c r="A14" s="1">
         <v>3250</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="10">
         <v>0.55800000000000005</v>
       </c>
     </row>
@@ -3071,7 +4208,7 @@
       <c r="A15" s="1">
         <v>3500</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="10">
         <v>0.495</v>
       </c>
     </row>
@@ -3079,7 +4216,7 @@
       <c r="A16" s="1">
         <v>3750</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="10">
         <v>0.47299999999999998</v>
       </c>
     </row>
@@ -3087,7 +4224,7 @@
       <c r="A17" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="10">
         <v>0.43</v>
       </c>
     </row>
@@ -3095,7 +4232,7 @@
       <c r="A18" s="1">
         <v>4250</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="10">
         <v>0.41299999999999998</v>
       </c>
     </row>
@@ -3103,7 +4240,7 @@
       <c r="A19" s="1">
         <v>4500</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="10">
         <v>0.39400000000000002</v>
       </c>
     </row>
@@ -3111,7 +4248,7 @@
       <c r="A20" s="1">
         <v>4750</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="10">
         <v>0.36599999999999999</v>
       </c>
     </row>
@@ -3119,7 +4256,7 @@
       <c r="A21" s="1">
         <v>5000</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="10">
         <v>0.36599999999999999</v>
       </c>
     </row>
@@ -3130,6 +4267,209 @@
       </c>
       <c r="B24" s="6">
         <v>0.91759999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.3109999999999999</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.306</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.294</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.306</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.3119999999999998</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.3069999999999999</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.31</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.3029999999999999</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.31</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.2949999999999999</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.2959999999999998</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.298</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.3029999999999999</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.29</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.3119999999999998</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6">
+        <v>8.3299999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>